<commit_message>
function to clear whitespaces
</commit_message>
<xml_diff>
--- a/processed/processed_2024.xlsx
+++ b/processed/processed_2024.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +482,46 @@
           <t>Cena</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Nazwa</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Opis</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Typ ostrza</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Moc silnika</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Typ silnika</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Typ zasilania</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -522,6 +562,46 @@
       <c r="H2" t="n">
         <v>300</v>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>EPT165PP</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>PODSTAWOWA PILARKA TARCZOWA, PRZEWODOWA - 165 MM, 800 W</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Podstawowa pilarka tarczowa do tarcz o rozmiarze 165 mm.</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>800 W</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>SZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>PRZEWODOWY</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -562,6 +642,46 @@
       <c r="H3" t="n">
         <v>500</v>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>EPT165UP</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>UNIWERSALNA PILARKA TARCZOWA, PRZEWODOWA - 165 MM, 1200 W</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Uniwersalna pilarka tarczowa do tarcz o rozmiarze 165 mm.</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1200 W</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>SZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>PRZEWODOWY</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>500.0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -602,6 +722,46 @@
       <c r="H4" t="n">
         <v>800</v>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>EPT165ZP</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>ZAAWANSOWANA PILARKA TARCZOWA, PRZEWODOWA - 165 MM, 1600 W</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Zaawansowana pilarka tarczowa do tarcz o rozmiarze 165 mm.</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>1600 W</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>BEZSZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>PRZEWODOWY</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>800.0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -642,6 +802,46 @@
       <c r="H5" t="n">
         <v>420</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>EPT165PA</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>PODSTAWOWA PILARKA TARCZOWA, AKUMULATOROWA - 165 MM, 800 W</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Podstawowa, akumulatorowa pilarka tarczowa do tarcz o rozmiarze 165 mm.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>800 W</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>SZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>AKUMULATOR 18V</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>420.0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -682,6 +882,46 @@
       <c r="H6" t="n">
         <v>650</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>EPT165UA</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>UNIWERSALNA PILARKA TARCZOWA, AKUMULATOROWA - 165 MM, 1200 W</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Uniwersalna, akumulatorowa pilarka tarczowa do tarcz o rozmiarze 165 mm.</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>1200 W</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>SZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>AKUMULATOR 18V</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>650.0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -722,6 +962,46 @@
       <c r="H7" t="n">
         <v>990</v>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>EPT165ZA</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>ZAAWANSOWANA PILARKA TARCZOWA, AKUMULATOROWA - 165 MM, 1600 W</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Zaawansowana, akumulatorowa pilarka tarczowa do tarcz o rozmiarze 165 mm.</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1600 W</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>BEZSZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>AKUMULATOR 18V</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>990.0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -762,6 +1042,46 @@
       <c r="H8" t="n">
         <v>320</v>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>EPSUP</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>UNIWERSALNA PIŁA SZABLASTA, 800 W</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Uniwersalna piła szablasta o mocy 800 W</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>800 W</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>SZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>PRZEWODOWY</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>320.0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -802,6 +1122,46 @@
       <c r="H9" t="n">
         <v>690</v>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>EPSZP</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>ZAAWANSOWANA PIŁA SZABLASTA, 1200 W</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Zaawansowana piła szablasta o mocy 1200 W</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>1200 W</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>BEZSZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>PRZEWODOWY</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>690.0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -842,6 +1202,46 @@
       <c r="H10" t="n">
         <v>520</v>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>EPSUA</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>UNIWERSALNA PIŁA SZABLASTA, AKUMULATOROWA , 800 W</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Uniwersalna piła szablasta o mocy 800 W, akumulatorowa</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>800 W</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>SZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>AKUMULATOR 18V</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>520.0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -881,6 +1281,46 @@
       </c>
       <c r="H11" t="n">
         <v>870</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>EPSZA</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>ZAAWANSOWANA PIŁA SZABLASTA, AKUMULATOROWA , 1200 W</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Zaawansowana piła szablasta o mocy 1200 W, akumulatorowa</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>1200 W</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>BEZSZCZOTKOWY</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>AKUMULATOR 18V</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>870.0</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -894,7 +1334,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -958,6 +1398,61 @@
           <t>Cena</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Nazwa</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Typ</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Opis</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Dlugosc</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Srednica</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Grubosc</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Material</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Liczba zebow (lub na cal)</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Zastosowanie</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1004,6 +1499,63 @@
       <c r="K2" t="n">
         <v>100</v>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>PTDP165</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA DO DREWNA - PODSTAWOWA 165</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Piła tarczowa o rozmiarze 165 mm do podstawowych zastowań przy drewnie.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>165.0</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>WĘGLIK SPIEKANY</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>DREWNO
+FORNIR
+PŁYTY WIÓROWE</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1050,6 +1602,63 @@
       <c r="K3" t="n">
         <v>180</v>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>PTDZ165</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA DO DREWNA - ZAAWANSOWANA 165</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Piła tarczowa do drewna o rozmiarze 165 mm  do najtrudniejszych zadań.</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>165.0</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>WĘGLIK SPIEKANY</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>DREWNO
+FORNIR
+PŁYTY WIÓROWE</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>180.0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1096,6 +1705,63 @@
       <c r="K4" t="n">
         <v>140</v>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PTDP210</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA DO DREWNA -  PODSTAWOWA 210</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Piła tarczowa o rozmiarze 210 mm  do podstawowych zastowań przy drewnie.</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>210.0</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>1.9</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>WĘGLIK SPIEKANY</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>DREWNO
+FORNIR
+PŁYTY WIÓROWE</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>140.0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1141,6 +1807,63 @@
       </c>
       <c r="K5" t="n">
         <v>220</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>PTDZ210</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA DO DREWNA - ZAAWANSOWANA 210</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Piła tarczowa do drewna  o rozmiarze 210 mm do najtrudniejszych zadań.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>210.0</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>1.9</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>WĘGLIK SPIEKANY</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>DREWNO
+FORNIR
+PŁYTY WIÓROWE</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>220.0</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -1189,43 +1912,52 @@
       <c r="K6" t="n">
         <v>210</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>PTU210</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>PIŁA TARCZOWA - UNIWERSALNA 210</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PTU165</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA - UNIWERSALNA 165</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>PIŁA TARCZOWA</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Uniwersalna piła tarczowa o rozmiarze 165 mm do roznych materiałów.</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>210</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="H7" t="inlineStr">
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>165.0</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
         <is>
           <t>WĘGLIK SPIEKANY</t>
         </is>
       </c>
-      <c r="I7" t="n">
-        <v>48</v>
-      </c>
-      <c r="J7" t="inlineStr">
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>48.0</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
         <is>
           <t>ALUMINIUM
 DREWNO
@@ -1233,8 +1965,115 @@
 PVC</t>
         </is>
       </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>210.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PTU210</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA - UNIWERSALNA 210</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Uniwersalna piła tarczowa o rozmiarze 165 mm do roznych materiałów.</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>210</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>WĘGLIK SPIEKANY</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>48</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>ALUMINIUM
+DREWNO
+LAMINAT
+PVC</t>
+        </is>
+      </c>
       <c r="K7" t="n">
         <v>270</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>PTU210</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA - UNIWERSALNA 210</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>PIŁA TARCZOWA</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Uniwersalna piła tarczowa o rozmiarze 165 mm do roznych materiałów.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>210.0</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>WĘGLIK SPIEKANY</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>48.0</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>ALUMINIUM
+DREWNO
+LAMINAT
+PVC</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>270.0</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1282,6 +2121,63 @@
       <c r="K8" t="n">
         <v>15</v>
       </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>BBM150</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY - DO METALU 150</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Brzeszczot bagnetowy do metalu o długości 150 mm.</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>150.0</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>HSS</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>LAMINAT
+METAL
+PVC</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1328,6 +2224,63 @@
       <c r="K9" t="n">
         <v>25</v>
       </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>BBM230</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY - DO METALU 230</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Brzeszczot bagnetowy do metalu o długości 230 mm.</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>230.0</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>HSS</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>LAMINAT
+METAL
+PVC</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1374,6 +2327,63 @@
       <c r="K10" t="n">
         <v>15</v>
       </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>BBD150</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY - DO DREWNA 150</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Brzeszczot bagnetowy do drewna o długości 150 mm.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>150.0</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>BIMETAL</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>DREWNO
+FORNIR
+PŁYTY WIÓROWE</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1420,6 +2430,63 @@
       <c r="K11" t="n">
         <v>25</v>
       </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>BBD230</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY - DO DREWNA 230</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Brzeszczot bagnetowy do drewna o długości 230 mm.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>230.0</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>BIMETAL</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>DREWNO
+FORNIR
+PŁYTY WIÓROWE</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1466,6 +2533,63 @@
       <c r="K12" t="n">
         <v>30</v>
       </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>BBM300</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY - DO METALU 300</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Brzeszczot bagnetowy do metalu o długości 300 mm.</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>230.0</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>HSS</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>LAMINAT
+METAL
+PVC</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>30.0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1511,6 +2635,63 @@
       </c>
       <c r="K13" t="n">
         <v>30</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>BBD300</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY - DO DREWNA 300</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>BRZESZCZOT BAGNETOWY</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Brzeszczot bagnetowy do drewna o długości 300 mm.</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>230.0</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>BIMETAL</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>DREWNO
+FORNIR
+PŁYTY WIÓROWE</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>30.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>